<commit_message>
state transition payments in C++
</commit_message>
<xml_diff>
--- a/examples/03_mortality/portfolio/portfolio_small_cli.xlsx
+++ b/examples/03_mortality/portfolio/portfolio_small_cli.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Oracle\PyProtolinc\examples\03_mortality\portfolio\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A71503-CB92-4AAE-A16A-1E3B2454E023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-420" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-420" windowWidth="29040" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -81,13 +75,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* \-??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -130,8 +124,8 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Dezimal" xfId="1" builtinId="3"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -189,7 +183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -241,7 +235,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -435,21 +429,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="A2" sqref="A2:L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.140625" customWidth="1"/>
@@ -462,7 +456,7 @@
     <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,21 +494,21 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>44561</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1">
-        <v>27873</v>
+        <v>22890</v>
       </c>
       <c r="D2" s="1">
-        <v>44562</v>
+        <v>42278</v>
       </c>
       <c r="E2" s="2">
-        <v>120000</v>
+        <v>100000</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -529,30 +523,30 @@
         <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K2">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="L2" s="1">
-        <v>44562</v>
+        <v>42278</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>44561</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>22890</v>
+        <v>27873</v>
       </c>
       <c r="D3" s="1">
-        <v>42278</v>
+        <v>44562</v>
       </c>
       <c r="E3" s="2">
-        <v>100000</v>
+        <v>120000</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -567,19 +561,14 @@
         <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K3">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="L3" s="1">
-        <v>42278</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+        <v>44562</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>